<commit_message>
added caps to bom
</commit_message>
<xml_diff>
--- a/mccoy/mccoy_bom.xlsx
+++ b/mccoy/mccoy_bom.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\polar\Documents\GitHub\scum-dev-board\mccoy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{96007F7A-784D-4C86-8F27-9615F9B9F171}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A112CC2-F26A-4266-99F1-FD1559270471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30705" yWindow="12150" windowWidth="13500" windowHeight="11505"/>
+    <workbookView xWindow="86280" yWindow="-120" windowWidth="18240" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mccoy_bom" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -80,12 +91,42 @@
   </si>
   <si>
     <t>CAP CER 0.1UF 6.3V 10% X7R 0402</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-electronics/GRM21BR60J107ME15L/6155751</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>CAP CER 100UF 6.3V X5R 0805</t>
+  </si>
+  <si>
+    <t>Murata Electronics</t>
+  </si>
+  <si>
+    <t>GRM21BR60J107ME15L</t>
+  </si>
+  <si>
+    <t>number of boards:</t>
+  </si>
+  <si>
+    <t>Price each @ 50</t>
+  </si>
+  <si>
+    <t>price tota</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/tdk-invensense/ICM-20948/6623535</t>
+  </si>
+  <si>
+    <t>C_1.1_OUT1, C_1.8_OUT2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
@@ -923,20 +964,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -959,13 +1004,28 @@
         <v>16</v>
       </c>
       <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>18</v>
       </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1">
+        <v>50</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -987,15 +1047,16 @@
       <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>3</v>
       </c>
-      <c r="I2">
-        <v>300</v>
-      </c>
-      <c r="N2" s="1"/>
+      <c r="J2">
+        <f>I2*$N$1</f>
+        <v>150</v>
+      </c>
+      <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1017,13 +1078,54 @@
       <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="J3">
+        <f>I3*$N$1</f>
+        <v>50</v>
+      </c>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <f>I4*$N$1</f>
         <v>100</v>
       </c>
-      <c r="N3" s="1"/>
+      <c r="K4">
+        <v>0.89739999999999998</v>
+      </c>
+      <c r="L4">
+        <f>K4*$N$1</f>
+        <v>44.87</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
brought bom up to date
</commit_message>
<xml_diff>
--- a/mccoy/mccoy_bom.xlsx
+++ b/mccoy/mccoy_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\polar\Documents\GitHub\scum-dev-board\mccoy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43C38B8-FE4C-45A1-A880-B6859B656A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380CF8A1-195C-43FF-9E9D-B9F896997159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -124,16 +124,56 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/mpd-memory-protection-devices/BK-870-TR/7918689</t>
+  </si>
+  <si>
+    <t>BATTERY RETAINER COIN 10MM SMD</t>
+  </si>
+  <si>
+    <t>BT1</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/renata-batteries/CR1025/13283207</t>
+  </si>
+  <si>
+    <t>BATTERY LITHIUM 3V COIN 10MM</t>
+  </si>
+  <si>
+    <t>Resistors for NRF_VDDD -&gt; VDDD divider</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/tdk-corporation/MLF1005G2R2JT000/4327831</t>
+  </si>
+  <si>
+    <t>FIXED IND 2.2UH 30MA 1.3 OHM SMD</t>
+  </si>
+  <si>
+    <t>C_1.1_IN1, C_1.8_IN2</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL05B104KQ5NNNC/3887169</t>
+  </si>
+  <si>
+    <t>R2, R3</t>
+  </si>
+  <si>
+    <t>L1, L2</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL05A106MP8NUB8/5961314</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 10V X5R 0402</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +304,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -566,7 +614,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -609,12 +657,16 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="43"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -642,12 +694,14 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="42" builtinId="4"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -968,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,6 +1036,9 @@
     <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="3"/>
+    <col min="14" max="14" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -1015,16 +1072,16 @@
       <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>25</v>
       </c>
-      <c r="N1">
+      <c r="O1">
         <v>50</v>
       </c>
     </row>
@@ -1050,12 +1107,22 @@
       <c r="G2" t="s">
         <v>4</v>
       </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
       <c r="I2">
         <v>3</v>
       </c>
       <c r="J2">
-        <f>I2*$N$1</f>
+        <f>I2*$O$1</f>
         <v>150</v>
+      </c>
+      <c r="K2" s="3">
+        <v>1.44E-2</v>
+      </c>
+      <c r="L2" s="3">
+        <f>K2*$O$1</f>
+        <v>0.72</v>
       </c>
       <c r="P2" s="1"/>
     </row>
@@ -1088,8 +1155,12 @@
         <v>1</v>
       </c>
       <c r="J3">
-        <f>I3*$N$1</f>
+        <f>I3*$O$1</f>
         <v>50</v>
+      </c>
+      <c r="L3" s="3">
+        <f>K3*$O$1</f>
+        <v>0</v>
       </c>
       <c r="P3" s="1"/>
     </row>
@@ -1119,23 +1190,269 @@
         <v>2</v>
       </c>
       <c r="J4">
-        <f>I4*$N$1</f>
+        <f>I4*$O$1</f>
         <v>100</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="3">
         <v>0.89739999999999998</v>
       </c>
-      <c r="L4">
-        <f>K4*$N$1</f>
+      <c r="L4" s="3">
+        <f>K4*$O$1</f>
         <v>44.87</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H5" t="s">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <f>I5*$O$1</f>
+        <v>50</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.63139999999999996</v>
+      </c>
+      <c r="L5" s="3">
+        <f>K5*$O$1</f>
+        <v>31.569999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <f>I6*$O$1</f>
+        <v>50</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="L6" s="3">
+        <f>K6*$O$1</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <f>I7*$O$1</f>
+        <v>100</v>
+      </c>
+      <c r="L7" s="3">
+        <f>K7*$O$1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <f>I8*$O$1</f>
+        <v>100</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="L8" s="3">
+        <f>K8*$O$1</f>
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <f>I9*$O$1</f>
+        <v>100</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.1804</v>
+      </c>
+      <c r="L9" s="3">
+        <f>K9*$O$1</f>
+        <v>9.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="J10">
+        <f>I10*$O$1</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="3">
+        <f>K10*$O$1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <f>I11*$O$1</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
+        <f>K11*$O$1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="J12">
+        <f>I12*$O$1</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
+        <f>K12*$O$1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H5" r:id="rId1" xr:uid="{F8A2CD34-5BB2-485B-A46D-EEE6238B341F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added OOS label to IMU :(
</commit_message>
<xml_diff>
--- a/mccoy/mccoy_bom.xlsx
+++ b/mccoy/mccoy_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\polar\Documents\GitHub\scum-dev-board\mccoy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226C6A75-D9CF-4746-BD7F-4BD341C15110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5843EEF-04AA-4188-832C-A9EAE0EED53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="86280" yWindow="-120" windowWidth="18240" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mccoy_bom" sheetId="1" r:id="rId1"/>
@@ -1027,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,47 +1409,51 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L20" s="3">
+        <f>SUM(L1:L19)</f>
+        <v>134.08000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>

</xml_diff>